<commit_message>
Refactored a ton of stuff because the template is wrong
</commit_message>
<xml_diff>
--- a/Projects/MILLERCOORS_SAND/Data/Miller Coors KPI Template_v1.xlsx
+++ b/Projects/MILLERCOORS_SAND/Data/Miller Coors KPI Template_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Adjacencies, Brands &amp; Segments" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,16 +17,32 @@
     <sheet name="Adjacency" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">KPIs!$A$1:$C$42</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$2:$E$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Print_Area_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">KPIs!$A$1:$C$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$2:$E$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="200">
   <si>
     <t xml:space="preserve">Next steps/Overall confirmations needed</t>
   </si>
@@ -574,15 +590,86 @@
     <t xml:space="preserve">Beer, Flavored Beer, Alcoholic Ciders and Alcoholic Malt Beverages - Cold Shelf (Open Deck Cooler)</t>
   </si>
   <si>
+    <t xml:space="preserve">Are the blocks for Miller Lite and Miller High Life Brands Adjacent in the cold section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are the blocks for Miller Lite and Miller High Life Brands Adjacent in the warm section?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beer, Flavored Beer, Alcoholic Ciders and Alcoholic Malt Beverages - Warm Shelf (Open Deck)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">any Coors Banquet beer adjacent to any Craft Segment beer?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">any Miller High Life beer adjacent to any Craft Segment beer?</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">a) Are Economy beers blocked in the cold section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b) When economy beers are blocked in the cold section, what brands are adjacent?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anchor</t>
   </si>
   <si>
     <t xml:space="preserve">Block</t>
   </si>
   <si>
+    <t xml:space="preserve">Sub Segment: Hard Sodas in cold section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Segment: Hard Sodas in warm section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand: Miller Lite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand: Miller High Life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand: Miller Genuine Draft</t>
+  </si>
+  <si>
     <t xml:space="preserve">param</t>
   </si>
   <si>
@@ -604,31 +691,13 @@
     <t xml:space="preserve">CRAFT</t>
   </si>
   <si>
-    <t xml:space="preserve">param1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">param2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Damn, Coney Island, Henry's, Not Your Father's, Not Your Father's Fruit Punch, Not Your Father's Ginger Ale, Not Your Father's Mountain Ale, Not Your Father's Root Beer, Not Your Father's Taproom, Not Your Father's Vanilla Cream Ale, Not Your Mom's Apple Pie, Not Your Mom's Iced Tea, Not Your Mom's Strawberry Rhubarb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bud Ice,Busch Ice,Camo Black,Camo,Icehouse,Icehouse Edge,Keystone Ice,Milwaukee's Best Ice,Natural Ice,Old Milwaukee Ice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Busch Light,Genny Light,Hamm's Special Light,I.C. Light,Keystone Light,Lone Star Light,Miller High Life Light,Milwaukee's Best Light,Natural Light,Old Milwaukee Light,Private Label,Southpaw Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blatz,Busch,Busch NA,Busch Signature,Camo Black,Colt 45,Coors Extra Gold,Dixie,Earthquake,Frio,Genesee,Hamm's,Hurricane,Keystone,King Cobra,Kul,Lone Star,Magnum,Mickeys,Miller High Life,Milwaukee's Best Lager,Narragansett,National Bohemian,Natty Daddy,Old Milwaukee,Old Style,Olympia,Pabst Blue Ribbon,Private Label,Rainier,Red Dog,Rhinelander,Rolling Rock,Schlitz,Stag,Steel Reserve 211,Stroh's,Utica Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miller Lite, Miller High Life, Miller Genuine Draft</t>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miller High Life</t>
   </si>
   <si>
     <t xml:space="preserve">anchor_param</t>
@@ -646,16 +715,7 @@
     <t xml:space="preserve">list_attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Miller High Life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beer &amp; Cider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brand_name</t>
+    <t xml:space="preserve">Hard Soda</t>
   </si>
   <si>
     <t xml:space="preserve">Michelob Ultra</t>
@@ -670,19 +730,16 @@
     <t xml:space="preserve">Miller LIte</t>
   </si>
   <si>
-    <t xml:space="preserve">subsegment</t>
-  </si>
-  <si>
     <t xml:space="preserve">CIDER</t>
   </si>
   <si>
     <t xml:space="preserve">Leinenkugel's</t>
   </si>
   <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
     <t xml:space="preserve">IMPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIllerCoors Segment</t>
   </si>
 </sst>
 </file>
@@ -693,7 +750,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -734,13 +791,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -814,7 +864,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -907,19 +957,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -927,32 +965,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1048,11 +1062,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.3074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,21 +1443,21 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.0814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.1444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="83.7851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.5074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="92.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2541,29 +2555,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="90.3518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="163.551851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="102.403703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.5074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="99.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="180.896296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="113.181481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,7 +2642,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>75</v>
@@ -2645,13 +2659,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,10 +2682,10 @@
         <v>75</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
         <v>6</v>
       </c>
@@ -2679,16 +2693,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
         <v>7</v>
       </c>
@@ -2696,71 +2710,75 @@
         <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="n">
+        <v>8</v>
+      </c>
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>96</v>
+      <c r="C11" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>99</v>
+      <c r="C12" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="n">
+        <v>11</v>
+      </c>
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>75</v>
@@ -2769,32 +2787,32 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="18" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>75</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>105</v>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>75</v>
@@ -2803,49 +2821,49 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="17" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>75</v>
@@ -2854,15 +2872,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>75</v>
@@ -2871,15 +2889,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>75</v>
@@ -2888,15 +2906,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>75</v>
@@ -2905,15 +2923,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>75</v>
@@ -2922,15 +2940,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>75</v>
@@ -2939,32 +2957,32 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="n">
-        <v>21</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>75</v>
@@ -2973,15 +2991,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="n">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>75</v>
@@ -2990,32 +3008,32 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="n">
-        <v>23</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>75</v>
@@ -3024,134 +3042,134 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E29" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="n">
-        <v>26</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="22" t="s">
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="n">
-        <v>27</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="n">
-        <v>29</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>75</v>
@@ -3160,32 +3178,32 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>75</v>
@@ -3194,15 +3212,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>75</v>
@@ -3211,15 +3229,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="n">
-        <v>36</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>153</v>
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>75</v>
@@ -3228,15 +3246,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="n">
-        <v>37</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>155</v>
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>175</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>75</v>
@@ -3245,25 +3263,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="n">
-        <v>38</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>161</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:E42"/>
+  <autoFilter ref="A2:E39"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3280,121 +3281,126 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="51.4481481481482"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="24.2037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="90.3518518518519"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="23" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="23" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.837037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="99.8555555555556"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="26"/>
+      <c r="B2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="26"/>
+      <c r="B3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>171</v>
+      <c r="B4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>168</v>
+      <c r="B6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>169</v>
+      <c r="B7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>171</v>
+      <c r="B8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3413,141 +3419,129 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="44.4888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+        <v>173</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3565,361 +3559,303 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="88.5851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="23" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="23" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="97.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.362962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="F5" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="F7" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="E12" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="23" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="C16" s="0" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="204.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="204.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="23" t="s">
+      <c r="D16" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="23" t="s">
+      <c r="B17" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3938,153 +3874,132 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="73.6925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="20.1666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="23" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.4333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="23" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="C6" s="0" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="D6" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>97</v>
+      <c r="F7" s="0" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of bug fixes and refactoring
</commit_message>
<xml_diff>
--- a/Projects/MILLERCOORS_SAND/Data/Miller Coors KPI Template_v1.xlsx
+++ b/Projects/MILLERCOORS_SAND/Data/Miller Coors KPI Template_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Adjacencies, Brands &amp; Segments" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,21 +28,29 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$1:$D$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'KPIs Reference'!$A$2:$I$42</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$C$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$2:$E$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="199">
   <si>
     <t xml:space="preserve">Next steps/Overall confirmations needed</t>
   </si>
@@ -691,6 +699,9 @@
     <t xml:space="preserve">CRAFT</t>
   </si>
   <si>
+    <t xml:space="preserve">Hard Soda</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
@@ -715,9 +726,6 @@
     <t xml:space="preserve">list_attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard Soda</t>
-  </si>
-  <si>
     <t xml:space="preserve">Michelob Ultra</t>
   </si>
   <si>
@@ -737,9 +745,6 @@
   </si>
   <si>
     <t xml:space="preserve">IMPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIllerCoors Segment</t>
   </si>
 </sst>
 </file>
@@ -1056,17 +1061,17 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.3074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.0518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.7555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,16 +1453,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.5074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="92.6037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="92.1148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="97.4074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,7 +2562,7 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -2567,17 +2572,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.5074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="99.8555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="180.896296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="113.181481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="92.1148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="105.048148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="190.403703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="119.062962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3284,17 +3289,17 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="99.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1023" min="5" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.6777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="105.048148148148"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,16 +3426,16 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.3888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.937037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,10 +3454,10 @@
         <v>171</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>183</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3460,10 +3465,10 @@
         <v>172</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>183</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,7 +3479,7 @@
         <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3485,7 +3490,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3496,7 +3501,7 @@
         <v>63</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,7 +3520,7 @@
         <v>173</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>25</v>
@@ -3526,10 +3531,10 @@
         <v>174</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,7 +3542,7 @@
         <v>175</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>30</v>
@@ -3567,12 +3572,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="97.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.796296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,19 +3585,19 @@
         <v>160</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,13 +3605,13 @@
         <v>162</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>25</v>
@@ -3617,13 +3622,13 @@
         <v>163</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>25</v>
@@ -3634,10 +3639,10 @@
         <v>96</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -3646,10 +3651,10 @@
         <v>99</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D5" s="3"/>
       <c r="F5" s="0" t="s">
@@ -3680,7 +3685,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +3693,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>192</v>
@@ -3705,13 +3710,13 @@
         <v>110</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>194</v>
@@ -3722,13 +3727,13 @@
         <v>113</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>194</v>
@@ -3739,13 +3744,13 @@
         <v>114</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>195</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>31</v>
@@ -3756,7 +3761,7 @@
         <v>115</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>37</v>
@@ -3773,7 +3778,7 @@
         <v>117</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>37</v>
@@ -3790,7 +3795,7 @@
         <v>122</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>197</v>
@@ -3807,7 +3812,7 @@
         <v>125</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>197</v>
@@ -3824,13 +3829,13 @@
         <v>127</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>41</v>
@@ -3841,13 +3846,13 @@
         <v>130</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>41</v>
@@ -3875,18 +3880,18 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.4333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="85.6481481481482"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3894,19 +3899,19 @@
         <v>160</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3914,13 +3919,13 @@
         <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>31</v>
@@ -3931,13 +3936,13 @@
         <v>80</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>192</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,7 +3964,7 @@
         <v>165</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>35</v>
@@ -3976,10 +3981,10 @@
         <v>166</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>181</v>
@@ -3999,7 +4004,7 @@
         <v>198</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>